<commit_message>
validar fecha actividad OK
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,7 +1730,7 @@
       <c r="AG4" s="2">
         <v>3</v>
       </c>
-      <c r="AH4" s="18">
+      <c r="AH4" s="17">
         <v>44479</v>
       </c>
       <c r="AI4" s="2">
@@ -1823,7 +1823,7 @@
       <c r="AG5" s="2">
         <v>1</v>
       </c>
-      <c r="AH5" s="18">
+      <c r="AH5" s="17">
         <v>44479</v>
       </c>
       <c r="AI5" s="2">

</xml_diff>

<commit_message>
update message validate date Ok
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
@@ -15,7 +15,7 @@
     <sheet name="3_BD_Gerencia Nacional FINAL" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3_BD_Gerencia Nacional FINAL'!$A$1:$AI$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3_BD_Gerencia Nacional FINAL'!$A$1:$AI$100</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="258">
   <si>
     <t>Edad</t>
   </si>
@@ -793,12 +793,6 @@
   </si>
   <si>
     <t>VALERIE</t>
-  </si>
-  <si>
-    <t>LORGIO</t>
-  </si>
-  <si>
-    <t>SUDARIO</t>
   </si>
   <si>
     <t>SC</t>
@@ -1306,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI101"/>
+  <dimension ref="A1:AI100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,10 +1351,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>10</v>
@@ -1417,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>28</v>
@@ -1435,7 +1429,7 @@
         <v>13</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AD1" s="12" t="s">
         <v>26</v>
@@ -1453,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="AI1" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -1461,7 +1455,7 @@
         <v>44479</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
@@ -1488,13 +1482,13 @@
         <v>215875848</v>
       </c>
       <c r="M2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N2" s="4">
         <v>74877886</v>
       </c>
       <c r="O2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -1508,7 +1502,7 @@
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V2" s="2">
         <v>25</v>
@@ -1517,13 +1511,13 @@
         <v>1</v>
       </c>
       <c r="X2" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y2" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z2" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="2">
         <v>2</v>
@@ -1535,20 +1529,18 @@
         <v>1</v>
       </c>
       <c r="AD2" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="AE2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF2" s="2">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="AG2" s="2">
-        <v>11</v>
-      </c>
-      <c r="AH2" s="17">
-        <v>44479</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="AH2" s="17"/>
       <c r="AI2" s="2">
         <v>1</v>
       </c>
@@ -1558,7 +1550,7 @@
         <v>44479</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
@@ -1649,7 +1641,7 @@
         <v>44479</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
@@ -1730,7 +1722,7 @@
       <c r="AG4" s="2">
         <v>3</v>
       </c>
-      <c r="AH4" s="17">
+      <c r="AH4" s="18">
         <v>44479</v>
       </c>
       <c r="AI4" s="2">
@@ -1742,7 +1734,7 @@
         <v>44479</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
@@ -1823,7 +1815,7 @@
       <c r="AG5" s="2">
         <v>1</v>
       </c>
-      <c r="AH5" s="17">
+      <c r="AH5" s="18">
         <v>44479</v>
       </c>
       <c r="AI5" s="2">
@@ -1835,7 +1827,7 @@
         <v>44479</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
@@ -1930,7 +1922,7 @@
         <v>44479</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
@@ -2023,7 +2015,7 @@
         <v>44479</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
@@ -2116,7 +2108,7 @@
         <v>44479</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
@@ -2209,7 +2201,7 @@
         <v>44479</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
@@ -2304,7 +2296,7 @@
         <v>44479</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
@@ -2399,7 +2391,7 @@
         <v>44479</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
@@ -2492,7 +2484,7 @@
         <v>44479</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
@@ -2589,7 +2581,7 @@
         <v>44479</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
@@ -2682,7 +2674,7 @@
         <v>44479</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
@@ -2779,7 +2771,7 @@
         <v>44479</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
@@ -2870,7 +2862,7 @@
         <v>44479</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
@@ -2965,7 +2957,7 @@
         <v>44479</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
@@ -3058,7 +3050,7 @@
         <v>44479</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
@@ -3153,7 +3145,7 @@
         <v>44479</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
@@ -3248,7 +3240,7 @@
         <v>44479</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
@@ -3341,7 +3333,7 @@
         <v>44479</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
@@ -3436,7 +3428,7 @@
         <v>44479</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
@@ -3531,7 +3523,7 @@
         <v>44479</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
@@ -3626,7 +3618,7 @@
         <v>44479</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
@@ -3721,7 +3713,7 @@
         <v>44479</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
@@ -3814,7 +3806,7 @@
         <v>44479</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
@@ -3907,7 +3899,7 @@
         <v>44479</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
@@ -4000,7 +3992,7 @@
         <v>44479</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1">
@@ -4093,7 +4085,7 @@
         <v>44479</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
@@ -4184,7 +4176,7 @@
         <v>44479</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1">
@@ -4277,7 +4269,7 @@
         <v>44479</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
@@ -4370,7 +4362,7 @@
         <v>44479</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1">
@@ -4465,7 +4457,7 @@
         <v>44479</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
@@ -4560,7 +4552,7 @@
         <v>44479</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1">
@@ -4653,7 +4645,7 @@
         <v>44479</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
@@ -4746,7 +4738,7 @@
         <v>44479</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1">
@@ -4843,7 +4835,7 @@
         <v>44479</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1">
@@ -4938,7 +4930,7 @@
         <v>44479</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1">
@@ -5033,7 +5025,7 @@
         <v>44479</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1">
@@ -5126,7 +5118,7 @@
         <v>44479</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1">
@@ -5221,7 +5213,7 @@
         <v>44479</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1">
@@ -5314,7 +5306,7 @@
         <v>44479</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1">
@@ -5411,7 +5403,7 @@
         <v>44479</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1">
@@ -5506,7 +5498,7 @@
         <v>44479</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1">
@@ -5601,7 +5593,7 @@
         <v>44479</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1">
@@ -5696,7 +5688,7 @@
         <v>44479</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1">
@@ -5787,7 +5779,7 @@
         <v>44479</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
@@ -5876,7 +5868,7 @@
         <v>44479</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1">
@@ -5963,7 +5955,7 @@
         <v>44479</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1">
@@ -6052,7 +6044,7 @@
         <v>44479</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1">
@@ -6147,7 +6139,7 @@
         <v>44479</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1">
@@ -6242,7 +6234,7 @@
         <v>44479</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1">
@@ -6333,7 +6325,7 @@
         <v>44479</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1">
@@ -6424,7 +6416,7 @@
         <v>44479</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1">
@@ -6519,7 +6511,7 @@
         <v>44479</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1">
@@ -6616,7 +6608,7 @@
         <v>44479</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1">
@@ -6709,7 +6701,7 @@
         <v>44479</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1">
@@ -6804,7 +6796,7 @@
         <v>44479</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1">
@@ -6899,7 +6891,7 @@
         <v>44479</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1">
@@ -6992,7 +6984,7 @@
         <v>44479</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1">
@@ -7085,7 +7077,7 @@
         <v>44479</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1">
@@ -7178,7 +7170,7 @@
         <v>44479</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1">
@@ -7273,7 +7265,7 @@
         <v>44479</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1">
@@ -7370,7 +7362,7 @@
         <v>44479</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1">
@@ -7461,7 +7453,7 @@
         <v>44479</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1">
@@ -7558,7 +7550,7 @@
         <v>44479</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1">
@@ -7655,7 +7647,7 @@
         <v>44479</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1">
@@ -7746,7 +7738,7 @@
         <v>44479</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1">
@@ -7837,7 +7829,7 @@
         <v>44479</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1">
@@ -7930,7 +7922,7 @@
         <v>44479</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1">
@@ -8023,7 +8015,7 @@
         <v>44479</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1">
@@ -8114,7 +8106,7 @@
         <v>44479</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1">
@@ -8205,7 +8197,7 @@
         <v>44479</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1">
@@ -8298,7 +8290,7 @@
         <v>44479</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1">
@@ -8393,7 +8385,7 @@
         <v>44479</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1">
@@ -8484,7 +8476,7 @@
         <v>44479</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1">
@@ -8581,7 +8573,7 @@
         <v>44479</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1">
@@ -8674,7 +8666,7 @@
         <v>44479</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1">
@@ -8767,7 +8759,7 @@
         <v>44479</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1">
@@ -8860,7 +8852,7 @@
         <v>44479</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1">
@@ -8951,7 +8943,7 @@
         <v>44479</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1">
@@ -9044,7 +9036,7 @@
         <v>44479</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1">
@@ -9139,7 +9131,7 @@
         <v>44479</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1">
@@ -9232,7 +9224,7 @@
         <v>44479</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1">
@@ -9325,7 +9317,7 @@
         <v>44479</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1">
@@ -9420,7 +9412,7 @@
         <v>44479</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1">
@@ -9513,7 +9505,7 @@
         <v>44479</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1">
@@ -9608,7 +9600,7 @@
         <v>44479</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1">
@@ -9703,7 +9695,7 @@
         <v>44479</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1">
@@ -9796,7 +9788,7 @@
         <v>44479</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1">
@@ -9887,7 +9879,7 @@
         <v>44479</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1">
@@ -9980,7 +9972,7 @@
         <v>44479</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1">
@@ -10071,7 +10063,7 @@
         <v>44479</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1">
@@ -10166,7 +10158,7 @@
         <v>44479</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1">
@@ -10259,7 +10251,7 @@
         <v>44479</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1">
@@ -10350,7 +10342,7 @@
         <v>44479</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1">
@@ -10441,7 +10433,7 @@
         <v>44479</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1">
@@ -10532,7 +10524,7 @@
         <v>44479</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1">
@@ -10625,7 +10617,7 @@
         <v>44479</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1">
@@ -10715,103 +10707,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A101" s="6">
-        <v>44479</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1">
-        <v>2021</v>
-      </c>
-      <c r="E101" s="2">
-        <v>1</v>
-      </c>
-      <c r="F101" s="1"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="I101" s="7"/>
-      <c r="J101" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K101" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="L101" s="7">
-        <v>218683284</v>
-      </c>
-      <c r="M101" s="2">
-        <v>1</v>
-      </c>
-      <c r="N101" s="8">
-        <v>80132087</v>
-      </c>
-      <c r="O101" s="2">
-        <v>1</v>
-      </c>
-      <c r="P101" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q101" s="3">
-        <v>2</v>
-      </c>
-      <c r="R101" s="2"/>
-      <c r="S101" s="7">
-        <v>983148489</v>
-      </c>
-      <c r="T101" s="2"/>
-      <c r="U101" s="9">
-        <v>2</v>
-      </c>
-      <c r="V101" s="7">
-        <v>59</v>
-      </c>
-      <c r="W101" s="2">
-        <v>1</v>
-      </c>
-      <c r="X101" s="3">
-        <v>2</v>
-      </c>
-      <c r="Y101" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z101" s="3">
-        <v>3</v>
-      </c>
-      <c r="AA101" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB101" s="2">
-        <v>10</v>
-      </c>
-      <c r="AC101" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD101" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE101" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF101" s="2">
-        <v>5</v>
-      </c>
-      <c r="AG101" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH101" s="18">
-        <v>44479</v>
-      </c>
-      <c r="AI101" s="2">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AI101"/>
+  <autoFilter ref="A1:AI100"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
update año y trimestre
automáticamente tabla Resultado proyectos
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1523,7 @@
         <v>2</v>
       </c>
       <c r="AB2" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC2" s="2">
         <v>1</v>
@@ -1540,7 +1540,9 @@
       <c r="AG2" s="2">
         <v>3</v>
       </c>
-      <c r="AH2" s="17"/>
+      <c r="AH2" s="17">
+        <v>44479</v>
+      </c>
       <c r="AI2" s="2">
         <v>1</v>
       </c>
@@ -1612,7 +1614,7 @@
         <v>2</v>
       </c>
       <c r="AB3" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC3" s="2">
         <v>1</v>
@@ -1705,7 +1707,7 @@
         <v>2</v>
       </c>
       <c r="AB4" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC4" s="2">
         <v>1</v>
@@ -1798,7 +1800,7 @@
         <v>2</v>
       </c>
       <c r="AB5" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC5" s="2">
         <v>1</v>
@@ -1893,7 +1895,7 @@
         <v>2</v>
       </c>
       <c r="AB6" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC6" s="2">
         <v>1</v>
@@ -1986,7 +1988,7 @@
         <v>2</v>
       </c>
       <c r="AB7" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC7" s="2">
         <v>1</v>
@@ -2079,7 +2081,7 @@
         <v>2</v>
       </c>
       <c r="AB8" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC8" s="2">
         <v>1</v>
@@ -2172,7 +2174,7 @@
         <v>2</v>
       </c>
       <c r="AB9" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC9" s="2">
         <v>1</v>
@@ -2267,7 +2269,7 @@
         <v>2</v>
       </c>
       <c r="AB10" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC10" s="2">
         <v>1</v>
@@ -2362,7 +2364,7 @@
         <v>2</v>
       </c>
       <c r="AB11" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC11" s="2">
         <v>1</v>
@@ -2455,7 +2457,7 @@
         <v>2</v>
       </c>
       <c r="AB12" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC12" s="2">
         <v>1</v>
@@ -2552,7 +2554,7 @@
         <v>2</v>
       </c>
       <c r="AB13" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC13" s="2">
         <v>1</v>
@@ -2645,7 +2647,7 @@
         <v>2</v>
       </c>
       <c r="AB14" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC14" s="2">
         <v>1</v>
@@ -2742,7 +2744,7 @@
         <v>2</v>
       </c>
       <c r="AB15" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC15" s="2">
         <v>1</v>
@@ -2833,7 +2835,7 @@
         <v>2</v>
       </c>
       <c r="AB16" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC16" s="2">
         <v>1</v>
@@ -2922,13 +2924,13 @@
         <v>1</v>
       </c>
       <c r="Z17" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA17" s="2">
         <v>2</v>
       </c>
       <c r="AB17" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC17" s="2">
         <v>1</v>
@@ -3021,7 +3023,7 @@
         <v>2</v>
       </c>
       <c r="AB18" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC18" s="2">
         <v>1</v>
@@ -3116,7 +3118,7 @@
         <v>2</v>
       </c>
       <c r="AB19" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC19" s="2">
         <v>1</v>
@@ -3205,13 +3207,13 @@
         <v>1</v>
       </c>
       <c r="Z20" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA20" s="2">
         <v>2</v>
       </c>
       <c r="AB20" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC20" s="2">
         <v>1</v>
@@ -3298,13 +3300,13 @@
         <v>3</v>
       </c>
       <c r="Z21" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA21" s="2">
         <v>2</v>
       </c>
       <c r="AB21" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC21" s="2">
         <v>1</v>
@@ -3399,7 +3401,7 @@
         <v>2</v>
       </c>
       <c r="AB22" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC22" s="2">
         <v>1</v>
@@ -3494,7 +3496,7 @@
         <v>2</v>
       </c>
       <c r="AB23" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC23" s="2">
         <v>1</v>
@@ -3589,7 +3591,7 @@
         <v>2</v>
       </c>
       <c r="AB24" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC24" s="2">
         <v>1</v>
@@ -3684,7 +3686,7 @@
         <v>2</v>
       </c>
       <c r="AB25" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC25" s="2">
         <v>1</v>
@@ -3777,7 +3779,7 @@
         <v>2</v>
       </c>
       <c r="AB26" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC26" s="2">
         <v>1</v>
@@ -3864,13 +3866,13 @@
         <v>2</v>
       </c>
       <c r="Z27" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA27" s="2">
         <v>2</v>
       </c>
       <c r="AB27" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC27" s="2">
         <v>1</v>
@@ -3963,7 +3965,7 @@
         <v>2</v>
       </c>
       <c r="AB28" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC28" s="2">
         <v>1</v>
@@ -4050,13 +4052,13 @@
         <v>3</v>
       </c>
       <c r="Z29" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA29" s="2">
         <v>2</v>
       </c>
       <c r="AB29" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC29" s="2">
         <v>1</v>
@@ -4147,7 +4149,7 @@
         <v>2</v>
       </c>
       <c r="AB30" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC30" s="2">
         <v>1</v>
@@ -4240,7 +4242,7 @@
         <v>2</v>
       </c>
       <c r="AB31" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC31" s="2">
         <v>1</v>
@@ -4333,7 +4335,7 @@
         <v>2</v>
       </c>
       <c r="AB32" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC32" s="2">
         <v>1</v>
@@ -4428,7 +4430,7 @@
         <v>2</v>
       </c>
       <c r="AB33" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC33" s="2">
         <v>1</v>
@@ -4523,7 +4525,7 @@
         <v>2</v>
       </c>
       <c r="AB34" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC34" s="2">
         <v>1</v>
@@ -4616,7 +4618,7 @@
         <v>2</v>
       </c>
       <c r="AB35" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC35" s="2">
         <v>1</v>
@@ -4709,7 +4711,7 @@
         <v>2</v>
       </c>
       <c r="AB36" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC36" s="2">
         <v>1</v>
@@ -4806,7 +4808,7 @@
         <v>2</v>
       </c>
       <c r="AB37" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC37" s="2">
         <v>1</v>
@@ -4901,7 +4903,7 @@
         <v>2</v>
       </c>
       <c r="AB38" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC38" s="2">
         <v>1</v>
@@ -4990,13 +4992,13 @@
         <v>1</v>
       </c>
       <c r="Z39" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA39" s="2">
         <v>2</v>
       </c>
       <c r="AB39" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC39" s="2">
         <v>1</v>
@@ -5089,7 +5091,7 @@
         <v>2</v>
       </c>
       <c r="AB40" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC40" s="2">
         <v>1</v>
@@ -5184,7 +5186,7 @@
         <v>2</v>
       </c>
       <c r="AB41" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC41" s="2">
         <v>1</v>
@@ -5277,7 +5279,7 @@
         <v>2</v>
       </c>
       <c r="AB42" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC42" s="2">
         <v>1</v>
@@ -5374,7 +5376,7 @@
         <v>2</v>
       </c>
       <c r="AB43" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC43" s="2">
         <v>1</v>
@@ -5469,7 +5471,7 @@
         <v>2</v>
       </c>
       <c r="AB44" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC44" s="2">
         <v>1</v>
@@ -5564,7 +5566,7 @@
         <v>2</v>
       </c>
       <c r="AB45" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC45" s="2">
         <v>1</v>
@@ -5659,7 +5661,7 @@
         <v>2</v>
       </c>
       <c r="AB46" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC46" s="2">
         <v>1</v>
@@ -5750,7 +5752,7 @@
         <v>2</v>
       </c>
       <c r="AB47" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC47" s="2">
         <v>1</v>
@@ -5839,7 +5841,7 @@
         <v>2</v>
       </c>
       <c r="AB48" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC48" s="2">
         <v>1</v>
@@ -5926,7 +5928,7 @@
         <v>2</v>
       </c>
       <c r="AB49" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC49" s="2">
         <v>1</v>
@@ -6015,7 +6017,7 @@
         <v>2</v>
       </c>
       <c r="AB50" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC50" s="2">
         <v>1</v>
@@ -6110,7 +6112,7 @@
         <v>2</v>
       </c>
       <c r="AB51" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC51" s="2">
         <v>1</v>
@@ -6205,7 +6207,7 @@
         <v>2</v>
       </c>
       <c r="AB52" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC52" s="2">
         <v>1</v>
@@ -6296,7 +6298,7 @@
         <v>2</v>
       </c>
       <c r="AB53" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC53" s="2">
         <v>1</v>
@@ -6387,7 +6389,7 @@
         <v>2</v>
       </c>
       <c r="AB54" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC54" s="2">
         <v>1</v>
@@ -6482,7 +6484,7 @@
         <v>2</v>
       </c>
       <c r="AB55" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC55" s="2">
         <v>1</v>
@@ -6573,13 +6575,13 @@
         <v>4</v>
       </c>
       <c r="Z56" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA56" s="2">
         <v>2</v>
       </c>
       <c r="AB56" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC56" s="2">
         <v>1</v>
@@ -6666,13 +6668,13 @@
         <v>1</v>
       </c>
       <c r="Z57" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA57" s="2">
         <v>2</v>
       </c>
       <c r="AB57" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC57" s="2">
         <v>1</v>
@@ -6767,7 +6769,7 @@
         <v>2</v>
       </c>
       <c r="AB58" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC58" s="2">
         <v>1</v>
@@ -6862,7 +6864,7 @@
         <v>2</v>
       </c>
       <c r="AB59" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC59" s="2">
         <v>1</v>
@@ -6949,13 +6951,13 @@
         <v>2</v>
       </c>
       <c r="Z60" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA60" s="2">
         <v>2</v>
       </c>
       <c r="AB60" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC60" s="2">
         <v>1</v>
@@ -7048,7 +7050,7 @@
         <v>2</v>
       </c>
       <c r="AB61" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC61" s="2">
         <v>1</v>
@@ -7141,7 +7143,7 @@
         <v>2</v>
       </c>
       <c r="AB62" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC62" s="2">
         <v>1</v>
@@ -7236,7 +7238,7 @@
         <v>2</v>
       </c>
       <c r="AB63" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC63" s="2">
         <v>1</v>
@@ -7333,7 +7335,7 @@
         <v>2</v>
       </c>
       <c r="AB64" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC64" s="2">
         <v>1</v>
@@ -7424,7 +7426,7 @@
         <v>2</v>
       </c>
       <c r="AB65" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC65" s="2">
         <v>1</v>
@@ -7515,13 +7517,13 @@
         <v>1</v>
       </c>
       <c r="Z66" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA66" s="2">
         <v>2</v>
       </c>
       <c r="AB66" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC66" s="2">
         <v>1</v>
@@ -7618,7 +7620,7 @@
         <v>2</v>
       </c>
       <c r="AB67" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC67" s="2">
         <v>1</v>
@@ -7709,7 +7711,7 @@
         <v>2</v>
       </c>
       <c r="AB68" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC68" s="2">
         <v>1</v>
@@ -7800,7 +7802,7 @@
         <v>2</v>
       </c>
       <c r="AB69" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC69" s="2">
         <v>1</v>
@@ -7893,7 +7895,7 @@
         <v>2</v>
       </c>
       <c r="AB70" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC70" s="2">
         <v>1</v>
@@ -7986,7 +7988,7 @@
         <v>2</v>
       </c>
       <c r="AB71" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC71" s="2">
         <v>1</v>
@@ -8077,7 +8079,7 @@
         <v>2</v>
       </c>
       <c r="AB72" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC72" s="2">
         <v>1</v>
@@ -8168,7 +8170,7 @@
         <v>2</v>
       </c>
       <c r="AB73" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC73" s="2">
         <v>1</v>
@@ -8261,7 +8263,7 @@
         <v>2</v>
       </c>
       <c r="AB74" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC74" s="2">
         <v>1</v>
@@ -8356,7 +8358,7 @@
         <v>2</v>
       </c>
       <c r="AB75" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC75" s="2">
         <v>1</v>
@@ -8441,13 +8443,13 @@
         <v>2</v>
       </c>
       <c r="Z76" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA76" s="2">
         <v>2</v>
       </c>
       <c r="AB76" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC76" s="2">
         <v>1</v>
@@ -8544,7 +8546,7 @@
         <v>2</v>
       </c>
       <c r="AB77" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC77" s="2">
         <v>1</v>
@@ -8637,7 +8639,7 @@
         <v>2</v>
       </c>
       <c r="AB78" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC78" s="2">
         <v>1</v>
@@ -8730,7 +8732,7 @@
         <v>2</v>
       </c>
       <c r="AB79" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC79" s="2">
         <v>1</v>
@@ -8817,13 +8819,13 @@
         <v>1</v>
       </c>
       <c r="Z80" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA80" s="2">
         <v>2</v>
       </c>
       <c r="AB80" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC80" s="2">
         <v>1</v>
@@ -8914,7 +8916,7 @@
         <v>2</v>
       </c>
       <c r="AB81" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC81" s="2">
         <v>1</v>
@@ -9007,7 +9009,7 @@
         <v>2</v>
       </c>
       <c r="AB82" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC82" s="2">
         <v>1</v>
@@ -9102,7 +9104,7 @@
         <v>2</v>
       </c>
       <c r="AB83" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC83" s="2">
         <v>1</v>
@@ -9189,13 +9191,13 @@
         <v>3</v>
       </c>
       <c r="Z84" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA84" s="2">
         <v>2</v>
       </c>
       <c r="AB84" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC84" s="2">
         <v>1</v>
@@ -9282,13 +9284,13 @@
         <v>1</v>
       </c>
       <c r="Z85" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA85" s="2">
         <v>2</v>
       </c>
       <c r="AB85" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC85" s="2">
         <v>1</v>
@@ -9383,7 +9385,7 @@
         <v>2</v>
       </c>
       <c r="AB86" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC86" s="2">
         <v>1</v>
@@ -9476,7 +9478,7 @@
         <v>2</v>
       </c>
       <c r="AB87" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC87" s="2">
         <v>1</v>
@@ -9571,7 +9573,7 @@
         <v>2</v>
       </c>
       <c r="AB88" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC88" s="2">
         <v>1</v>
@@ -9660,13 +9662,13 @@
         <v>2</v>
       </c>
       <c r="Z89" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA89" s="2">
         <v>2</v>
       </c>
       <c r="AB89" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC89" s="2">
         <v>1</v>
@@ -9753,13 +9755,13 @@
         <v>2</v>
       </c>
       <c r="Z90" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA90" s="2">
         <v>2</v>
       </c>
       <c r="AB90" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC90" s="2">
         <v>1</v>
@@ -9850,7 +9852,7 @@
         <v>2</v>
       </c>
       <c r="AB91" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC91" s="2">
         <v>1</v>
@@ -9943,7 +9945,7 @@
         <v>2</v>
       </c>
       <c r="AB92" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC92" s="2">
         <v>1</v>
@@ -10034,7 +10036,7 @@
         <v>2</v>
       </c>
       <c r="AB93" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC93" s="2">
         <v>1</v>
@@ -10129,7 +10131,7 @@
         <v>2</v>
       </c>
       <c r="AB94" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC94" s="2">
         <v>1</v>
@@ -10222,7 +10224,7 @@
         <v>2</v>
       </c>
       <c r="AB95" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC95" s="2">
         <v>1</v>
@@ -10313,7 +10315,7 @@
         <v>2</v>
       </c>
       <c r="AB96" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC96" s="2">
         <v>1</v>
@@ -10404,7 +10406,7 @@
         <v>2</v>
       </c>
       <c r="AB97" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC97" s="2">
         <v>1</v>
@@ -10489,13 +10491,13 @@
         <v>4</v>
       </c>
       <c r="Z98" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA98" s="2">
         <v>2</v>
       </c>
       <c r="AB98" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC98" s="2">
         <v>1</v>
@@ -10588,7 +10590,7 @@
         <v>2</v>
       </c>
       <c r="AB99" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC99" s="2">
         <v>1</v>
@@ -10683,7 +10685,7 @@
         <v>2</v>
       </c>
       <c r="AB100" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC100" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
update page migracion 01
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Z27" sqref="Z27"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1538,7 @@
         <v>4</v>
       </c>
       <c r="AG2" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AH2" s="17">
         <v>44479</v>
@@ -1632,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="AH3" s="17">
-        <v>44479</v>
+        <v>44114</v>
       </c>
       <c r="AI3" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
update page migracion 02
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos.xlsx
@@ -1303,7 +1303,7 @@
   <dimension ref="A1:AI100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="AH3" s="17">
-        <v>44114</v>
+        <v>44479</v>
       </c>
       <c r="AI3" s="2">
         <v>1</v>

</xml_diff>